<commit_message>
Todos os exercicios finalizados e adicionados banco de dados DML e DQL
</commit_message>
<xml_diff>
--- a/1.3-exercicio-pclinics/1.3-exercicio-pclinics-excel.xlsx
+++ b/1.3-exercicio-pclinics/1.3-exercicio-pclinics-excel.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23821"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23822"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2D6A8DAA-B571-4C07-9C54-5857950743C1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{1575459D-D572-485E-AE49-532F1AE2FD1C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,26 +26,29 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="56">
   <si>
     <t>Clinica</t>
   </si>
   <si>
+    <t>Dono</t>
+  </si>
+  <si>
     <t>Veterinario</t>
   </si>
   <si>
+    <t>tipoPet</t>
+  </si>
+  <si>
     <t>Raça</t>
   </si>
   <si>
+    <t>Pet</t>
+  </si>
+  <si>
     <t>Atendimento</t>
   </si>
   <si>
-    <t>Pet</t>
-  </si>
-  <si>
-    <t>Dono</t>
-  </si>
-  <si>
     <t>idClinica</t>
   </si>
   <si>
@@ -58,6 +61,18 @@
     <t>TelefoneClinica</t>
   </si>
   <si>
+    <t>idDono</t>
+  </si>
+  <si>
+    <t>NomeDono</t>
+  </si>
+  <si>
+    <t>Idade</t>
+  </si>
+  <si>
+    <t>TelefoneDono</t>
+  </si>
+  <si>
     <t>idVeterinario</t>
   </si>
   <si>
@@ -67,7 +82,7 @@
     <t>CRM</t>
   </si>
   <si>
-    <t>Idade</t>
+    <t>idTipoPet</t>
   </si>
   <si>
     <t>idRaca</t>
@@ -76,7 +91,13 @@
     <t>Nome</t>
   </si>
   <si>
-    <t>idTipoPet</t>
+    <t>idPet</t>
+  </si>
+  <si>
+    <t>NomePet</t>
+  </si>
+  <si>
+    <t>DataNascimento</t>
   </si>
   <si>
     <t>idAtendimento</t>
@@ -91,39 +112,39 @@
     <t>Data</t>
   </si>
   <si>
-    <t>idPet</t>
-  </si>
-  <si>
-    <t>NomePet</t>
-  </si>
-  <si>
-    <t>DataNascimento</t>
-  </si>
-  <si>
-    <t>idDono</t>
-  </si>
-  <si>
-    <t>NomeDono</t>
-  </si>
-  <si>
-    <t>TelefoneDono</t>
-  </si>
-  <si>
     <t>R.Arroz Doce, 48</t>
   </si>
   <si>
     <t>Amor ao Pet</t>
   </si>
   <si>
+    <t>(11) 94567-8988</t>
+  </si>
+  <si>
+    <t>Luiza</t>
+  </si>
+  <si>
+    <t>(11) 98765-4738</t>
+  </si>
+  <si>
     <t>Lais</t>
   </si>
   <si>
     <t>A054008</t>
   </si>
   <si>
+    <t>Cachorro</t>
+  </si>
+  <si>
     <t>Pinscher</t>
   </si>
   <si>
+    <t>Lilica</t>
+  </si>
+  <si>
+    <t>01/06/2013</t>
+  </si>
+  <si>
     <t>7h30</t>
   </si>
   <si>
@@ -133,19 +154,46 @@
     <t>24/02/2021</t>
   </si>
   <si>
-    <t>Lilica</t>
-  </si>
-  <si>
-    <t>01/06/2013</t>
-  </si>
-  <si>
-    <t>Luiza</t>
+    <t>R.Goiabada, 87</t>
+  </si>
+  <si>
+    <t>Clinica do amor</t>
+  </si>
+  <si>
+    <t>(11) 94567-7626</t>
+  </si>
+  <si>
+    <t>Mauricio</t>
+  </si>
+  <si>
+    <t>(11) 94729-8382</t>
   </si>
   <si>
     <t>Tonia</t>
   </si>
   <si>
     <t>A054007</t>
+  </si>
+  <si>
+    <t>Gato</t>
+  </si>
+  <si>
+    <t>Hamster</t>
+  </si>
+  <si>
+    <t>Meg</t>
+  </si>
+  <si>
+    <t>07/07/2019</t>
+  </si>
+  <si>
+    <t>16h43</t>
+  </si>
+  <si>
+    <t>Infecção urinária</t>
+  </si>
+  <si>
+    <t>23/09/2020</t>
   </si>
 </sst>
 </file>
@@ -161,7 +209,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="17">
+  <fills count="19">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -255,6 +303,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFAEAAAA"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA9D08E"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA6A6A6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -271,45 +331,30 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1"/>
@@ -317,6 +362,30 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="16" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="18" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -633,249 +702,363 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AE4"/>
+  <dimension ref="A1:AI5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="U1" workbookViewId="0">
-      <selection activeCell="AB3" sqref="AB3:AE3"/>
+    <sheetView tabSelected="1" topLeftCell="T1" workbookViewId="0">
+      <selection activeCell="AH8" sqref="AH8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="20.42578125" customWidth="1"/>
-    <col min="18" max="18" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="18" width="10.85546875" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="13" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="15.85546875" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="14" bestFit="1" customWidth="1"/>
+    <col min="30" max="31" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:35">
+      <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="F1" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
-      <c r="K1" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="L1" s="7"/>
-      <c r="M1" s="7"/>
-      <c r="O1" s="10" t="s">
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="F1" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" s="12"/>
+      <c r="H1" s="12"/>
+      <c r="I1" s="12"/>
+      <c r="K1" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="L1" s="13"/>
+      <c r="M1" s="13"/>
+      <c r="N1" s="13"/>
+      <c r="O1" s="13"/>
+      <c r="Q1" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="P1" s="10"/>
-      <c r="Q1" s="10"/>
-      <c r="R1" s="10"/>
-      <c r="S1" s="10"/>
-      <c r="T1" s="10"/>
-      <c r="V1" s="13" t="s">
+      <c r="R1" s="13"/>
+      <c r="T1" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="W1" s="13"/>
-      <c r="X1" s="13"/>
-      <c r="Y1" s="13"/>
-      <c r="Z1" s="13"/>
-      <c r="AB1" s="1" t="s">
+      <c r="U1" s="14"/>
+      <c r="V1" s="14"/>
+      <c r="X1" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="AC1" s="1"/>
-      <c r="AD1" s="1"/>
-      <c r="AE1" s="1"/>
+      <c r="Y1" s="16"/>
+      <c r="Z1" s="16"/>
+      <c r="AA1" s="16"/>
+      <c r="AB1" s="16"/>
+      <c r="AD1" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="AE1" s="15"/>
+      <c r="AF1" s="15"/>
+      <c r="AG1" s="15"/>
+      <c r="AH1" s="15"/>
+      <c r="AI1" s="15"/>
     </row>
-    <row r="2" spans="1:31">
-      <c r="A2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" s="2" t="s">
+    <row r="2" spans="1:35">
+      <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="C2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="D2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="F2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="G2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="I2" s="5" t="s">
+      <c r="H2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="K2" s="8" t="s">
+      <c r="I2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="L2" s="8" t="s">
+      <c r="K2" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="M2" s="8" t="s">
+      <c r="L2" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="O2" s="11" t="s">
+      <c r="M2" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="P2" s="11" t="s">
+      <c r="N2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="O2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q2" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="Q2" s="11" t="s">
+      <c r="R2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="T2" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="R2" s="11" t="s">
+      <c r="U2" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="S2" s="11" t="s">
+      <c r="V2" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="X2" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="T2" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="V2" s="14" t="s">
+      <c r="Y2" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="Z2" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="AA2" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="AB2" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="AD2" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="AE2" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="AF2" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="AG2" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="AH2" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="W2" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="X2" s="14" t="s">
+      <c r="AI2" s="7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:35">
+      <c r="A3" s="2">
+        <v>1</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F3" s="2">
+        <v>1</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="H3" s="2">
+        <v>57</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="K3" s="4">
+        <v>1</v>
+      </c>
+      <c r="L3" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="M3" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="N3" s="4">
+        <v>38</v>
+      </c>
+      <c r="O3" s="4">
+        <v>1</v>
+      </c>
+      <c r="Q3" s="17">
+        <v>1</v>
+      </c>
+      <c r="R3" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="T3" s="6">
+        <v>1</v>
+      </c>
+      <c r="U3" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="V3" s="6">
+        <v>1</v>
+      </c>
+      <c r="X3" s="10">
+        <v>1</v>
+      </c>
+      <c r="Y3" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="Z3" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="AA3" s="10">
+        <v>1</v>
+      </c>
+      <c r="AB3" s="10">
+        <v>1</v>
+      </c>
+      <c r="AD3" s="8">
+        <v>1</v>
+      </c>
+      <c r="AE3" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="AF3" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="AG3" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="AH3" s="8">
+        <v>1</v>
+      </c>
+      <c r="AI3" s="8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:35">
+      <c r="A4" s="2">
+        <v>2</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="F4" s="2">
+        <v>2</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="H4" s="2">
         <v>23</v>
       </c>
-      <c r="Y2" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="Z2" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="AB2" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="AC2" s="2" t="s">
+      <c r="I4" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="K4" s="4">
+        <v>2</v>
+      </c>
+      <c r="L4" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="M4" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="N4" s="4">
         <v>25</v>
       </c>
-      <c r="AD2" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="AE2" s="2" t="s">
-        <v>26</v>
+      <c r="O4" s="4">
+        <v>2</v>
+      </c>
+      <c r="Q4" s="17">
+        <v>2</v>
+      </c>
+      <c r="R4" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="T4" s="6">
+        <v>2</v>
+      </c>
+      <c r="U4" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="V4" s="6">
+        <v>3</v>
+      </c>
+      <c r="X4" s="18">
+        <v>2</v>
+      </c>
+      <c r="Y4" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z4" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA4" s="18">
+        <v>2</v>
+      </c>
+      <c r="AB4" s="18">
+        <v>2</v>
+      </c>
+      <c r="AD4" s="8">
+        <v>2</v>
+      </c>
+      <c r="AE4" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="AF4" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="AG4" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="AH4" s="8">
+        <v>2</v>
+      </c>
+      <c r="AI4" s="8">
+        <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:31">
-      <c r="A3" s="3">
-        <v>1</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="D3" s="3">
-        <v>945678988</v>
-      </c>
-      <c r="F3" s="6">
-        <v>1</v>
-      </c>
-      <c r="G3" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="H3" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="I3" s="6">
-        <v>38</v>
-      </c>
-      <c r="K3" s="9">
-        <v>1</v>
-      </c>
-      <c r="L3" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="M3" s="9">
-        <v>2</v>
-      </c>
-      <c r="O3" s="12">
-        <v>1</v>
-      </c>
-      <c r="P3" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q3" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="R3" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="S3" s="12">
-        <v>1</v>
-      </c>
-      <c r="T3" s="12">
-        <v>2</v>
-      </c>
-      <c r="V3" s="15">
-        <v>1</v>
-      </c>
-      <c r="W3" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="X3" s="16" t="s">
-        <v>36</v>
-      </c>
-      <c r="Y3" s="15">
-        <v>1</v>
-      </c>
-      <c r="Z3" s="15">
-        <v>1</v>
-      </c>
-      <c r="AB3" s="3">
-        <v>1</v>
-      </c>
-      <c r="AC3" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="AD3" s="3">
-        <v>57</v>
-      </c>
-      <c r="AE3" s="3">
-        <v>987654738</v>
-      </c>
-    </row>
-    <row r="4" spans="1:31">
-      <c r="F4" s="6">
-        <v>2</v>
-      </c>
-      <c r="G4" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="H4" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="I4" s="6">
-        <v>25</v>
+    <row r="5" spans="1:35">
+      <c r="Q5" s="17">
+        <v>3</v>
+      </c>
+      <c r="R5" s="17" t="s">
+        <v>50</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="7">
+    <mergeCell ref="F1:I1"/>
+    <mergeCell ref="Q1:R1"/>
+    <mergeCell ref="K1:O1"/>
     <mergeCell ref="A1:D1"/>
-    <mergeCell ref="F1:I1"/>
-    <mergeCell ref="K1:M1"/>
-    <mergeCell ref="O1:T1"/>
-    <mergeCell ref="V1:Z1"/>
-    <mergeCell ref="AB1:AE1"/>
+    <mergeCell ref="T1:V1"/>
+    <mergeCell ref="AD1:AI1"/>
+    <mergeCell ref="X1:AB1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>